<commit_message>
Auto-committed on 2023/03/03 週五 11:41:27.01
</commit_message>
<xml_diff>
--- a/Program/Other/LM033_底稿_新撥案件明細.xlsx
+++ b/Program/Other/LM033_底稿_新撥案件明細.xlsx
@@ -1,35 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\iTX\Other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855F34C0-53C0-4212-80DA-3EB1590CB03D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
   </bookViews>
   <sheets>
     <sheet name="D9701211" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">D9701211!$A$1:$N$88</definedName>
-    <definedName name="_xlnm.Database">D9701211!$A$1:$N$88</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">D9701211!$A$1:$M$88</definedName>
+    <definedName name="_xlnm.Database">D9701211!$A$1:$M$88</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>放款部放款管理課張舜雯</author>
   </authors>
   <commentList>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -114,11 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t xml:space="preserve">單位別    </t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">申請日期    </t>
     <phoneticPr fontId="19" type="noConversion"/>
@@ -143,26 +138,26 @@
     <t xml:space="preserve">   循環動用期限</t>
   </si>
   <si>
-    <t xml:space="preserve">代號 1   </t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
     <t>核貸利率</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
-    <t>企金別1</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
     <t>計件代碼</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
+  <si>
+    <t xml:space="preserve">擔保品代號1   </t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>企金別</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="0.0000"/>
@@ -170,7 +165,7 @@
     <numFmt numFmtId="178" formatCode="#,##0_ "/>
     <numFmt numFmtId="179" formatCode="#,##0.00_ "/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -350,6 +345,13 @@
       <color indexed="81"/>
       <name val="細明體"/>
       <family val="3"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="標楷體"/>
+      <family val="4"/>
       <charset val="136"/>
     </font>
     <font>
@@ -794,36 +796,42 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="23" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="24" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -960,23 +968,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1012,23 +1003,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1204,80 +1178,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="20.81640625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="13.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.90625" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.90625" style="7"/>
+    <col min="1" max="1" width="15.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="20.81640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="13.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.90625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="8">
+        <f>SUBTOTAL(3,C2:C1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3">
-        <f>SUBTOTAL(3,D2:D1048576)</f>
+      <c r="E1" s="9">
+        <f>SUBTOTAL(9,E2:E1048576)</f>
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4">
+      <c r="F1" s="9">
         <f>SUBTOTAL(9,F2:F1048576)</f>
         <v>0</v>
       </c>
-      <c r="G1" s="4">
-        <f>SUBTOTAL(9,G2:G1048576)</f>
-        <v>0</v>
+      <c r="G1" s="10" t="s">
+        <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="6" t="s">
+      <c r="L1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>10</v>
+      <c r="M1" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N88" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:M88"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>